<commit_message>
Atualizar Calculador de Médias
</commit_message>
<xml_diff>
--- a/Average Calculator.xlsx
+++ b/Average Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\MIEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64834140-439C-413D-9090-0A51A2E74D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0D4062-BF3C-4BFA-AE4E-5A784623AB1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,6 +561,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,30 +604,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1850,7 +1850,7 @@
   </sheetPr>
   <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -1869,11 +1869,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G3" s="29">
+      <c r="G3" s="37">
         <f>F4/F5</f>
         <v>13.351351351351351</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E4" s="19" t="s">
@@ -1883,8 +1883,8 @@
         <f>SUM(C16:H16,C20:H20,C26:H26,C30:H30,C36:H36,C40:H40,C46:H46,C50:H50,C56,C60)</f>
         <v>2470</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="19" t="s">
@@ -1894,12 +1894,12 @@
         <f>SUM(C15:H15,C19:H19,D25:H25,D29:H29,C35:H35,C39:F39,H39,E45:H45)</f>
         <v>185</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
@@ -1911,7 +1911,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +1959,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1983,7 +1983,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
@@ -2013,7 +2013,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
@@ -2061,7 +2061,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
@@ -2662,10 +2662,10 @@
       <c r="B47" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="36"/>
+      <c r="D47" s="34"/>
       <c r="E47" s="10" t="s">
         <v>30</v>
       </c>
@@ -2683,10 +2683,10 @@
       <c r="B48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="37">
+      <c r="C48" s="36">
         <v>0</v>
       </c>
-      <c r="D48" s="37"/>
+      <c r="D48" s="36"/>
       <c r="E48" s="11">
         <v>0</v>
       </c>
@@ -2704,10 +2704,10 @@
       <c r="B49" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="36">
         <v>10</v>
       </c>
-      <c r="D49" s="37"/>
+      <c r="D49" s="36"/>
       <c r="E49" s="11">
         <v>5</v>
       </c>
@@ -2725,11 +2725,11 @@
       <c r="B50" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="32">
         <f xml:space="preserve"> C48*C49</f>
         <v>0</v>
       </c>
-      <c r="D50" s="40"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="12">
         <f t="shared" ref="E50" si="27" xml:space="preserve"> E48*E49</f>
         <v>0</v>
@@ -2769,124 +2769,124 @@
       <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
     </row>
     <row r="54" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="42">
+      <c r="C54" s="30">
         <v>0</v>
       </c>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
     </row>
     <row r="55" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="31">
         <v>15</v>
       </c>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
     </row>
     <row r="56" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B56" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="33">
         <f xml:space="preserve"> C54*C55</f>
         <v>0</v>
       </c>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="38"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
     </row>
     <row r="57" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C57" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
     </row>
     <row r="58" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B58" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="39">
+      <c r="C58" s="35">
         <v>0</v>
       </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
     </row>
     <row r="59" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B59" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="37">
+      <c r="C59" s="36">
         <v>45</v>
       </c>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
     </row>
     <row r="60" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B60" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="40">
+      <c r="C60" s="32">
         <f xml:space="preserve"> C58*C59</f>
         <v>0</v>
       </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C57:H57"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="G3:H6"/>
     <mergeCell ref="C53:H53"/>
     <mergeCell ref="C54:H54"/>
     <mergeCell ref="C55:H55"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C56:H56"/>
-    <mergeCell ref="C57:H57"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="C59:H59"/>
-    <mergeCell ref="C60:H60"/>
-    <mergeCell ref="G3:H6"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2901,7 +2901,7 @@
   </sheetPr>
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -2920,11 +2920,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G3" s="29">
+      <c r="G3" s="37">
         <f>F4/F5</f>
         <v>12.053571428571429</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E4" s="19" t="s">
@@ -2934,8 +2934,8 @@
         <f>(1*(H14+D14+C14+G14+C17+E17+G17+F17+H22+C22+F25+G25)+1.5*(E14+H17+G22+F22+D25+E30+F30+F33)+2*(F14+D17+D22+E22+C25+E25+H25+C30+D30+G30+H30+C33+D33+E33+H33+G33))</f>
         <v>675</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="19" t="s">
@@ -2944,12 +2944,12 @@
       <c r="F5" s="18">
         <v>56</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
@@ -2961,7 +2961,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="9" t="s">
         <v>52</v>
       </c>
@@ -3057,7 +3057,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
@@ -3081,7 +3081,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -3115,7 +3115,7 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
+      <c r="A20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">

</xml_diff>

<commit_message>
Adicionar TP3 VI II
</commit_message>
<xml_diff>
--- a/Average Calculator.xlsx
+++ b/Average Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\MIEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6621D1BE-38F0-4646-B917-634E7E39A214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17090F89-7FD7-4AE6-A3CA-7C29AC34DF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Média Portal Académico" sheetId="5" r:id="rId1"/>
@@ -1850,8 +1850,8 @@
   </sheetPr>
   <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1871,7 +1871,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G3" s="34">
         <f>F4/F5</f>
-        <v>13.351351351351351</v>
+        <v>13.842105263157896</v>
       </c>
       <c r="H3" s="35"/>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="F4" s="18">
         <f>SUM(C16:H16,C20:H20,C26:H26,C30:H30,C36:H36,C40:H40,C46:H46,C50:H50,C56,C60)</f>
-        <v>2470</v>
+        <v>2630</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="37"/>
@@ -1891,8 +1891,8 @@
         <v>55</v>
       </c>
       <c r="F5" s="18">
-        <f>SUM(C15:H15,C19:H19,D25:H25,D29:H29,C35:H35,C39:F39,H39,E45:H45)</f>
-        <v>185</v>
+        <f>SUM(C15:H15,C19:H19,D25:H25,D29:H29,C35:H35,C39:G39,H39,E45:H45)</f>
+        <v>190</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="37"/>
@@ -2484,7 +2484,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H38" s="11">
         <v>16</v>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="G40" s="12">
         <f t="shared" ref="G40" si="20" xml:space="preserve"> G38*G39</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H40" s="12">
         <f t="shared" ref="H40" si="21" xml:space="preserve"> H38*H39</f>
@@ -2691,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="11">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G48" s="11">
         <v>0</v>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="F50" s="12">
         <f t="shared" ref="F50" si="28" xml:space="preserve"> F48*F49</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G50" s="12">
         <f t="shared" ref="G50" si="29" xml:space="preserve"> G48*G49</f>
@@ -2901,7 +2901,7 @@
   </sheetPr>
   <dimension ref="A2:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mudanças de nomes Pastas
</commit_message>
<xml_diff>
--- a/Average Calculator.xlsx
+++ b/Average Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\MIEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17090F89-7FD7-4AE6-A3CA-7C29AC34DF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38250B22-5D25-4D99-8403-8CF0BEAF6504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,49 +561,49 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1850,8 +1850,8 @@
   </sheetPr>
   <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1869,11 +1869,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G3" s="34">
+      <c r="G3" s="32">
         <f>F4/F5</f>
-        <v>13.842105263157896</v>
-      </c>
-      <c r="H3" s="35"/>
+        <v>14.236842105263158</v>
+      </c>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E4" s="19" t="s">
@@ -1881,10 +1881,10 @@
       </c>
       <c r="F4" s="18">
         <f>SUM(C16:H16,C20:H20,C26:H26,C30:H30,C36:H36,C40:H40,C46:H46,C50:H50,C56,C60)</f>
-        <v>2630</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
+        <v>2705</v>
+      </c>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="19" t="s">
@@ -1894,12 +1894,12 @@
         <f>SUM(C15:H15,C19:H19,D25:H25,D29:H29,C35:H35,C39:G39,H39,E45:H45)</f>
         <v>190</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
@@ -1911,7 +1911,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +1959,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1983,7 +1983,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
@@ -2013,7 +2013,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
@@ -2061,7 +2061,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
@@ -2662,10 +2662,10 @@
       <c r="B47" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="30"/>
+      <c r="D47" s="43"/>
       <c r="E47" s="10" t="s">
         <v>30</v>
       </c>
@@ -2683,10 +2683,10 @@
       <c r="B48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="31">
+      <c r="C48" s="30">
         <v>0</v>
       </c>
-      <c r="D48" s="31"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="11">
         <v>0</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>17</v>
       </c>
       <c r="G48" s="11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H48" s="11">
         <v>0</v>
@@ -2704,10 +2704,10 @@
       <c r="B49" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="31">
+      <c r="C49" s="30">
         <v>10</v>
       </c>
-      <c r="D49" s="31"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="11">
         <v>5</v>
       </c>
@@ -2725,11 +2725,11 @@
       <c r="B50" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="33">
+      <c r="C50" s="31">
         <f xml:space="preserve"> C48*C49</f>
         <v>0</v>
       </c>
-      <c r="D50" s="33"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="12">
         <f t="shared" ref="E50" si="27" xml:space="preserve"> E48*E49</f>
         <v>0</v>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="G50" s="12">
         <f t="shared" ref="G50" si="29" xml:space="preserve"> G48*G49</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H50" s="12">
         <f t="shared" ref="H50" si="30" xml:space="preserve"> H48*H49</f>
@@ -2769,110 +2769,115 @@
       <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
     </row>
     <row r="54" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="41">
+      <c r="C54" s="39">
         <v>0</v>
       </c>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
     </row>
     <row r="55" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="42">
+      <c r="C55" s="40">
         <v>15</v>
       </c>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
     </row>
     <row r="56" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B56" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="41">
         <f xml:space="preserve"> C54*C55</f>
         <v>0</v>
       </c>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
     </row>
     <row r="57" spans="2:8" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C57" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
     </row>
     <row r="58" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B58" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="32">
+      <c r="C58" s="29">
         <v>0</v>
       </c>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
     </row>
     <row r="59" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B59" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="31">
+      <c r="C59" s="30">
         <v>45</v>
       </c>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
     </row>
     <row r="60" spans="2:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B60" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="33">
+      <c r="C60" s="31">
         <f xml:space="preserve"> C58*C59</f>
         <v>0</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C57:H57"/>
     <mergeCell ref="C58:H58"/>
     <mergeCell ref="C59:H59"/>
     <mergeCell ref="C60:H60"/>
@@ -2882,11 +2887,6 @@
     <mergeCell ref="C55:H55"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C56:H56"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C57:H57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2920,11 +2920,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G3" s="34">
+      <c r="G3" s="32">
         <f>F4/F5</f>
         <v>11.589285714285714</v>
       </c>
-      <c r="H3" s="35"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E4" s="19" t="s">
@@ -2934,8 +2934,8 @@
         <f>(1*(H14+D14+C14+G14+C17+E17+G17+F17+H22+C22+F25+G25)+1.5*(E14+H17+G22+F22+D25+E30+F30+F33)+2*(F14+D17+D22+E22+C25+E25+H25+C30+D30+G30+H30+C33+D33+E33+H33+G33))</f>
         <v>649</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="19" t="s">
@@ -2944,12 +2944,12 @@
       <c r="F5" s="18">
         <v>56</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
@@ -2961,7 +2961,7 @@
       <c r="H10" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="9" t="s">
         <v>52</v>
       </c>
@@ -3057,7 +3057,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
@@ -3081,7 +3081,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -3115,7 +3115,7 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
+      <c r="A20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="27" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">

</xml_diff>